<commit_message>
automate software and current work pages
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15560" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="620" yWindow="0" windowWidth="25540" windowHeight="15560" tabRatio="500" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="teaching" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="mentorship" sheetId="4" r:id="rId5"/>
     <sheet name="experience" sheetId="5" r:id="rId6"/>
     <sheet name="affiliations" sheetId="6" r:id="rId7"/>
-    <sheet name="affiliations2" sheetId="8" r:id="rId8"/>
+    <sheet name="current_work" sheetId="8" r:id="rId8"/>
+    <sheet name="software" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="284">
   <si>
     <t>data</t>
   </si>
@@ -712,6 +713,184 @@
   </si>
   <si>
     <t>San Luis Obispo California</t>
+  </si>
+  <si>
+    <t>main</t>
+  </si>
+  <si>
+    <t>sub</t>
+  </si>
+  <si>
+    <t>working_with</t>
+  </si>
+  <si>
+    <t>pic</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>ET</t>
+  </si>
+  <si>
+    <t>Evapotranspiration Data Analysis</t>
+  </si>
+  <si>
+    <t>Dami Eyelade, Jeremy Neill, Dino Korac</t>
+  </si>
+  <si>
+    <t>resources/images/current_work/et.png</t>
+  </si>
+  <si>
+    <t>Four projects look into modeling evapotranspiration across a continuous spatial surface within the contexts of the HydroData package. Specifically (1) how DAYMET and Weather Underground data can be used to calculate PET at a daily timesteps for North America; (2) how the same process can be applied globally; (4) how values – analogous to the FAO crop coefficients – can be developed for all vegetated Anderson level 2 land covers and (4) how to decouple the effect of temperature on ET rates using observed streamflow records.</t>
+  </si>
+  <si>
+    <t>Flood Mapping</t>
+  </si>
+  <si>
+    <t>Jim Coll, Dinuke Munasinghe</t>
+  </si>
+  <si>
+    <t>resources/images/current_work/floodmapping.gif</t>
+  </si>
+  <si>
+    <t>Three projects look at the feasibility of real-time flood mapping using R and the National Water Model. The first (1) is to develop a system that allows GIS agencies throughout the country to install and run an hourly flood impacts models using the HAND methodology, the second (2) is to evaluate the accuracy of the HAND method against a repository of satellite derived flood extents and the third (3) is develop a filtering scheme to identify abnormally low and high flows in a NWM forecast allowing decision-makers and modelers to focus on areas that need attention.</t>
+  </si>
+  <si>
+    <t>Water Security</t>
+  </si>
+  <si>
+    <t>Using Text-based Analysis to Simplify the Water Security Paradigm</t>
+  </si>
+  <si>
+    <t>Keith Clarke</t>
+  </si>
+  <si>
+    <t>Over the last 25 years the concept of water security has gained in popularity, but its meaning remains ambiguous despite several attempts to articulate a unified definition. This project seeks to better understand water security through a quantitative, text-based analysis of the literature to remove linguistic redundancies and overlap to identify core, timeless agreements.</t>
+  </si>
+  <si>
+    <t>resources/images/current_work/watersecurity.jpg</t>
+  </si>
+  <si>
+    <t>Urban Growth Modeling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This study looks to apply the SLEUTH land use/land cover model to the state of California to derive high resolution, probabilistic, long-range, Anderson level 2 land use products. Such products will be used for scenario-based hydroclimate studies with the NCAR Research Application Laboratory. </t>
+  </si>
+  <si>
+    <t>resources/images/current_work/urbangrowth.jpg</t>
+  </si>
+  <si>
+    <t>Agent-based Risk Models</t>
+  </si>
+  <si>
+    <t>Drought Models</t>
+  </si>
+  <si>
+    <t>Marthe Wens, Jeroen Aerts, Ted Veldkamp</t>
+  </si>
+  <si>
+    <t>This work is part of a larger study being carried out at the Institute for Environmental Studies at VU Amsterdam looking to couple distributed hydrologic models and multi-actor, agent-based behavioral models within a drought risk context. One case study looks at applying this modeling strategy to a region in California’s Central Valley to better understand impacts on ground water withdrawals and aquifer levels.</t>
+  </si>
+  <si>
+    <t>resources/images/current_work/droughtmodels.jpg</t>
+  </si>
+  <si>
+    <t>AOI</t>
+  </si>
+  <si>
+    <t>HydroData</t>
+  </si>
+  <si>
+    <t>FlowFinder</t>
+  </si>
+  <si>
+    <t>NWM</t>
+  </si>
+  <si>
+    <t>nwmViewer</t>
+  </si>
+  <si>
+    <t>Area of Interest</t>
+  </si>
+  <si>
+    <t>Hydrology as a Service</t>
+  </si>
+  <si>
+    <t>An R client for the National Water Model</t>
+  </si>
+  <si>
+    <t>Vizualize National Water Model Output</t>
+  </si>
+  <si>
+    <t>If you’ve ever found yourself needing to geocode or reverse geocode a location, formalize an area of interest, get bounding geometries, decribe a place by lat/long, or better understand spatial locations this package should be able to help.
+An area of interest (AOI) is a geographic extent. It helps confine and formalize a unit of work to a geographic area, and prioritize and define research and sub setting efforts while improving reproducibility. They are built around concrete spatail attributes but often are discussed in a more colloquail way. The aim of the is package is to help make the colloquial understanding of space more concrete.</t>
+  </si>
+  <si>
+    <t>Almost all environmental research begins with data; the question of what data is available; and the challenge of gathering it. HydroData is an R package designed to help users find, get, visualize and use a range of Earth Systems data for a defined Area of Interest. The package provides functions to automatically download data from 19 sources; interactively visualize and share data within R and/or a browser; and to export data for external use in GIS.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FlowFinder provides access to five-day out streamflow forecasts at a three hour time step for all of CONUS and visualizes data for a 225 square mile region centered on a users requested location (area of interest: AOI). Areas of exceedingly high flow - when compared to long term normals are marked and mapped throughout CONUS, and AOI metadata is provided. </t>
+  </si>
+  <si>
+    <t>Each day the NOAA NWM produces ~400 GB of forecast data for the CONUS. This data is stored for a 40 day rolling window on the HydroShare Thredds server amounting to over 16,000 GB (2 TB) of data being stored and accessible at any one time. This package aims to provide access to this data in a clean, fast, and convenient way through the R environment.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nwmViewer is an R Shiny application built to quickly find and vizualize data via the nwm package. </t>
+  </si>
+  <si>
+    <t>resources/images/software/aoi.png</t>
+  </si>
+  <si>
+    <t>resources/images/software/hydrodata.png</t>
+  </si>
+  <si>
+    <t>resources/images/software/flowfinder.png</t>
+  </si>
+  <si>
+    <t>resources/images/software/nwm.png</t>
+  </si>
+  <si>
+    <t>resources/images/software/nwmViewer.png</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://overdodactyl.github.io"&gt;Pat Johnson&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>https://mikejohnson51.github.io/AOI/</t>
+  </si>
+  <si>
+    <t>https://github.com/mikejohnson51/AOI</t>
+  </si>
+  <si>
+    <t>https://mikejohnson51.github.io/HydroData/</t>
+  </si>
+  <si>
+    <t>https://github.com/mikejohnson51/HydroData</t>
+  </si>
+  <si>
+    <t>https://mikejohnson51.github.io/FlowFinder/</t>
+  </si>
+  <si>
+    <t>https://github.com/mikejohnson51/FlowFinder</t>
+  </si>
+  <si>
+    <t>https://mikejohnson51.github.io/NWM/</t>
+  </si>
+  <si>
+    <t>ttps://github.com/mikejohnson51/NWM</t>
+  </si>
+  <si>
+    <t>https://github.com/overdodactyl/nwmViewer</t>
+  </si>
+  <si>
+    <t>https://nwmviewer.shinyapps.io/view/</t>
+  </si>
+  <si>
+    <t>homepage</t>
+  </si>
+  <si>
+    <t>app</t>
   </si>
 </sst>
 </file>
@@ -773,11 +952,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
   </cellXfs>
@@ -1334,7 +1516,7 @@
     <col min="4" max="4" width="163.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="63.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="4"/>
+    <col min="8" max="8" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -1359,7 +1541,7 @@
       <c r="G1" t="s">
         <v>185</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="5" t="s">
         <v>184</v>
       </c>
       <c r="I1" t="s">
@@ -1385,10 +1567,10 @@
       <c r="E2" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="I2" s="4"/>
+      <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -1403,7 +1585,7 @@
       <c r="D3" t="s">
         <v>153</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="5" t="s">
         <v>215</v>
       </c>
     </row>
@@ -1426,7 +1608,7 @@
       <c r="G4" t="s">
         <v>188</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="5" t="s">
         <v>189</v>
       </c>
     </row>
@@ -1452,7 +1634,7 @@
       <c r="G5" t="s">
         <v>191</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="5" t="s">
         <v>192</v>
       </c>
     </row>
@@ -1478,7 +1660,7 @@
       <c r="G6" t="s">
         <v>193</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="5" t="s">
         <v>194</v>
       </c>
     </row>
@@ -1501,7 +1683,7 @@
       <c r="G7" t="s">
         <v>188</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="5" t="s">
         <v>195</v>
       </c>
     </row>
@@ -1581,7 +1763,7 @@
       <c r="G11" t="s">
         <v>202</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="5" t="s">
         <v>203</v>
       </c>
     </row>
@@ -1604,7 +1786,7 @@
       <c r="G12" t="s">
         <v>202</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="5" t="s">
         <v>204</v>
       </c>
     </row>
@@ -2053,8 +2235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2294,7 +2476,7 @@
       <c r="F10" s="3">
         <v>50</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="6" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2308,12 +2490,270 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="144" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D2" t="s">
+        <v>233</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="160" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D3" t="s">
+        <v>237</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="96" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>239</v>
+      </c>
+      <c r="B4" t="s">
+        <v>240</v>
+      </c>
+      <c r="C4" t="s">
+        <v>241</v>
+      </c>
+      <c r="D4" t="s">
+        <v>243</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="80" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>244</v>
+      </c>
+      <c r="C5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D5" t="s">
+        <v>246</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="112" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>248</v>
+      </c>
+      <c r="B6" t="s">
+        <v>247</v>
+      </c>
+      <c r="C6" t="s">
+        <v>249</v>
+      </c>
+      <c r="D6" t="s">
+        <v>251</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>250</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54" style="4" customWidth="1"/>
+    <col min="6" max="6" width="38" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="F1" t="s">
+        <v>282</v>
+      </c>
+      <c r="G1" t="s">
+        <v>186</v>
+      </c>
+      <c r="H1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="176" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B2" t="s">
+        <v>257</v>
+      </c>
+      <c r="D2" t="s">
+        <v>266</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="F2" t="s">
+        <v>272</v>
+      </c>
+      <c r="G2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>253</v>
+      </c>
+      <c r="D3" t="s">
+        <v>267</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="F3" t="s">
+        <v>274</v>
+      </c>
+      <c r="G3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>254</v>
+      </c>
+      <c r="B4" t="s">
+        <v>258</v>
+      </c>
+      <c r="C4" t="s">
+        <v>271</v>
+      </c>
+      <c r="D4" t="s">
+        <v>268</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="F4" t="s">
+        <v>276</v>
+      </c>
+      <c r="G4" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>255</v>
+      </c>
+      <c r="B5" t="s">
+        <v>259</v>
+      </c>
+      <c r="D5" t="s">
+        <v>269</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="F5" t="s">
+        <v>278</v>
+      </c>
+      <c r="G5" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>256</v>
+      </c>
+      <c r="B6" t="s">
+        <v>260</v>
+      </c>
+      <c r="C6" t="s">
+        <v>271</v>
+      </c>
+      <c r="D6" t="s">
+        <v>270</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="G6" t="s">
+        <v>280</v>
+      </c>
+      <c r="H6" t="s">
+        <v>281</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
spelling errors and formatting
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patjohnson/Documents/GitHub/mike_johnson/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5D0DA3-C3DD-A24D-9EF1-CC5BD17EE9EF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A8CAD39-ED0B-9C49-947B-81BDBB516C22}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="teaching" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="322">
   <si>
     <t>data</t>
   </si>
@@ -110,60 +110,33 @@
     <t>Travel Grant (AGU)</t>
   </si>
   <si>
-    <t>Graduate Student Association (\$200)</t>
-  </si>
-  <si>
     <t>Summer Research Grant</t>
   </si>
   <si>
-    <t>UCSB Geography (\$2,400)</t>
-  </si>
-  <si>
     <t>COMET Partners Grant</t>
   </si>
   <si>
-    <t>UCAR (\$15,000)</t>
-  </si>
-  <si>
     <t>Seed Grant</t>
   </si>
   <si>
-    <t>UCGHI Planetary Health Center (\$10,000)</t>
-  </si>
-  <si>
     <t>Travel Scholarship (AGU)</t>
   </si>
   <si>
-    <t>Dangermond Fund (\$800)</t>
-  </si>
-  <si>
     <t>National Water Center Course Coordinator</t>
   </si>
   <si>
-    <t>CUASHI (\$15,000)</t>
-  </si>
-  <si>
     <t>Travel Grant (WRF-Hydro Training)</t>
   </si>
   <si>
-    <t>CUASHI (\$500)</t>
-  </si>
-  <si>
     <t>Travel Grant (HAZUS Conference)</t>
   </si>
   <si>
-    <t>Dangermond Fund (\$700)</t>
-  </si>
-  <si>
     <t>2015-2016</t>
   </si>
   <si>
     <t>Disciplines Fellowship</t>
   </si>
   <si>
-    <t>University of California Regents (\$30,000)</t>
-  </si>
-  <si>
     <t>Outstanding Senior</t>
   </si>
   <si>
@@ -171,9 +144,6 @@
   </si>
   <si>
     <t>Top undergraduate paper</t>
-  </si>
-  <si>
-    <t>California Geographical Society (\$500)</t>
   </si>
   <si>
     <t>authors</t>
@@ -452,9 +422,6 @@
     <t>July 2017</t>
   </si>
   <si>
-    <t>CUASHI Hydroinformatics Conference</t>
-  </si>
-  <si>
     <t>Real-time Discharge-to-Damage Flood Mapping 'Anywhere, USA'</t>
   </si>
   <si>
@@ -506,9 +473,6 @@
     <t>July 2016</t>
   </si>
   <si>
-    <t>CUASHI Biennial Conference</t>
-  </si>
-  <si>
     <t>Densified Radar Measurement and Flow Modeling</t>
   </si>
   <si>
@@ -677,13 +641,7 @@
     <t>https://www.ivm.vu.nl/en/index.aspx</t>
   </si>
   <si>
-    <t>CUASHI</t>
-  </si>
-  <si>
     <t>Cambridge Massachusetts</t>
-  </si>
-  <si>
-    <t>../resources/images/affiliations/cuashi.png</t>
   </si>
   <si>
     <t>https://www.cuahsi.org/</t>
@@ -1000,6 +958,51 @@
   </si>
   <si>
     <t>An R Package for flood mapping (HAND &amp; National Water Model)</t>
+  </si>
+  <si>
+    <t>Graduate Student Association ($200)</t>
+  </si>
+  <si>
+    <t>UCSB Geography ($2,400)</t>
+  </si>
+  <si>
+    <t>UCAR ($15,000)</t>
+  </si>
+  <si>
+    <t>UCGHI Planetary Health Center ($10,000)</t>
+  </si>
+  <si>
+    <t>Dangermond Fund ($800)</t>
+  </si>
+  <si>
+    <t>Dangermond Fund ($700)</t>
+  </si>
+  <si>
+    <t>University of California Regents ($30,000)</t>
+  </si>
+  <si>
+    <t>California Geographical Society ($500)</t>
+  </si>
+  <si>
+    <t>CUAHSI ($15,000)</t>
+  </si>
+  <si>
+    <t>CUAHSI ($500)</t>
+  </si>
+  <si>
+    <t>https://github.com/mikejohnson51/nwmRetro</t>
+  </si>
+  <si>
+    <t>CUAHSI Hydroinformatics Conference</t>
+  </si>
+  <si>
+    <t>CUAHSI Biennial Conference</t>
+  </si>
+  <si>
+    <t>CUAHSI</t>
+  </si>
+  <si>
+    <t>../resources/images/affiliations/CUAHSI.png</t>
   </si>
 </sst>
 </file>
@@ -1606,8 +1609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView zoomScale="44" zoomScaleNormal="44" workbookViewId="0">
-      <selection activeCell="B12" activeCellId="1" sqref="I8 B12"/>
+    <sheetView zoomScale="108" zoomScaleNormal="44" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1637,7 +1640,7 @@
         <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>307</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1645,10 +1648,10 @@
         <v>2018</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>308</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1656,10 +1659,10 @@
         <v>2018</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>309</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1667,10 +1670,10 @@
         <v>2017</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>310</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1678,10 +1681,10 @@
         <v>2017</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>311</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1689,10 +1692,10 @@
         <v>2017</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>315</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1700,10 +1703,10 @@
         <v>2017</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>316</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1711,21 +1714,21 @@
         <v>2016</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>312</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>42</v>
+        <v>313</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1733,10 +1736,10 @@
         <v>2015</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1744,10 +1747,10 @@
         <v>2015</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -1780,296 +1783,296 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
         <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="G1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="I1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="J1" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
         <v>57</v>
       </c>
-      <c r="C4" t="s">
-        <v>67</v>
-      </c>
       <c r="D4" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B5">
         <v>2018</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E5" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="G5" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B6">
         <v>2018</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D6" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E6" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="F6" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="G6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B7">
         <v>2017</v>
       </c>
       <c r="C7" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="D7" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E7" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F7" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="G7" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B8">
         <v>2017</v>
       </c>
       <c r="C8" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D8" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E8" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="G8" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B9">
         <v>2017</v>
       </c>
       <c r="C9" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D9" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="I9" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="J9" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B10">
         <v>2017</v>
       </c>
       <c r="C10" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="D10" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="I10" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="J10" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B11">
         <v>2017</v>
       </c>
       <c r="C11" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="D11" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="E11" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="I11" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="J11" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B12">
         <v>2016</v>
       </c>
       <c r="C12" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="D12" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="E12" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="G12" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="B13">
         <v>2016</v>
       </c>
       <c r="C13" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="D13" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="E13" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="G13" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -2085,8 +2088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView zoomScale="44" zoomScaleNormal="44" workbookViewId="0">
-      <selection activeCell="D21" activeCellId="1" sqref="I8 D21"/>
+    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="44" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2103,237 +2106,237 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C2" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D2" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B3" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="D3" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C4" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="D4" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B5" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C5" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="D5" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B6" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="C6" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="D6" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="B7" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="D7" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B8" t="s">
-        <v>138</v>
+        <v>318</v>
       </c>
       <c r="C8" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="D8" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="B9" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="C9" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="D9" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="B10" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="C10" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="D10" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="B11" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="C11" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="D11" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="B12" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="C12" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="D12" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="B13" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="C13" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="D13" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="B14" t="s">
-        <v>156</v>
+        <v>319</v>
       </c>
       <c r="C14" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="D14" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="B15" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C15" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="D15" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="B16" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="C16" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="D16" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="B17" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="C17" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="D17" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="19" x14ac:dyDescent="0.2">
@@ -2365,7 +2368,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B1" t="s">
         <v>22</v>
@@ -2373,18 +2376,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="B2" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="B3" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -2392,7 +2395,7 @@
         <v>2017</v>
       </c>
       <c r="B4" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -2422,10 +2425,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -2433,10 +2436,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="C2" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2444,32 +2447,32 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="C3" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="B4" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="C4" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="B5" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="C5" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2477,10 +2480,10 @@
         <v>2017</v>
       </c>
       <c r="B6" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="C6" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2488,10 +2491,10 @@
         <v>2017</v>
       </c>
       <c r="B7" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="C7" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2499,10 +2502,10 @@
         <v>2016</v>
       </c>
       <c r="B8" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="C8" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2510,10 +2513,10 @@
         <v>2016</v>
       </c>
       <c r="B9" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="C9" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -2521,21 +2524,21 @@
         <v>2015</v>
       </c>
       <c r="B10" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="C10" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="B11" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="C11" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -2543,10 +2546,10 @@
         <v>2014</v>
       </c>
       <c r="B12" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="C12" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -2554,10 +2557,10 @@
         <v>2013</v>
       </c>
       <c r="B13" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="C13" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -2588,33 +2591,33 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="C2" s="4">
         <v>-119.845</v>
@@ -2623,21 +2626,21 @@
         <v>34.414999999999999</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="F2" s="4">
         <v>75</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="C3" s="4">
         <v>4.8657000000000004</v>
@@ -2646,21 +2649,21 @@
         <v>52.333799999999997</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="F3" s="4">
         <v>75</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>213</v>
+        <v>320</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="C4" s="4">
         <v>-71.109700000000004</v>
@@ -2669,21 +2672,21 @@
         <v>42.373600000000003</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>215</v>
+        <v>321</v>
       </c>
       <c r="F4" s="4">
         <v>50</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="C5" s="4">
         <v>-77.306399999999996</v>
@@ -2692,21 +2695,21 @@
         <v>38.846200000000003</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="F5" s="4">
         <v>75</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="C6" s="4">
         <v>-87.541399999999996</v>
@@ -2715,21 +2718,21 @@
         <v>33.217599999999997</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="F6" s="4">
         <v>50</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="C7" s="4">
         <v>-105.27500000000001</v>
@@ -2738,21 +2741,21 @@
         <v>39.978299999999997</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="F7" s="4">
         <v>50</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="C8" s="4">
         <v>-122.4586</v>
@@ -2761,21 +2764,21 @@
         <v>37.762700000000002</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="F8" s="4">
         <v>75</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="C9" s="4">
         <v>-122.2711</v>
@@ -2784,21 +2787,21 @@
         <v>37.804400000000001</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="F9" s="4">
         <v>50</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="C10" s="4">
         <v>-120.66249999999999</v>
@@ -2807,13 +2810,13 @@
         <v>35.305</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="F10" s="4">
         <v>50</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -2845,98 +2848,98 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="B1" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="C1" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="D1" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="153" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="B2" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="D2" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="170" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="C3" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="D3" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="B4" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="C4" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="D4" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="C5" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="D5" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="B6" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="C6" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="D6" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -2949,8 +2952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2970,215 +2973,217 @@
   <sheetData>
     <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="404" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="306" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="306" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="153" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="85" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>302</v>
+        <v>288</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="204" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>285</v>
-      </c>
-      <c r="G9" s="14"/>
+        <v>271</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>317</v>
+      </c>
       <c r="I9" s="12" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update cv and website
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patjohnson/Documents/GitHub/mike_johnson/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikejohnson/Documents/GitHub/mikejohnson51/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29925BD2-6301-194A-A0CD-0FF7421D3ABE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC32B6E-23F8-2E45-AC0D-3E7348F3066A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="teaching" sheetId="1" r:id="rId1"/>
     <sheet name="awards" sheetId="2" r:id="rId2"/>
-    <sheet name="publications" sheetId="3" r:id="rId3"/>
-    <sheet name="presentations" sheetId="4" r:id="rId4"/>
-    <sheet name="mentorship" sheetId="5" r:id="rId5"/>
-    <sheet name="experience" sheetId="6" r:id="rId6"/>
-    <sheet name="affiliations" sheetId="7" r:id="rId7"/>
-    <sheet name="current_work" sheetId="8" r:id="rId8"/>
-    <sheet name="software" sheetId="9" r:id="rId9"/>
+    <sheet name="evaluations" sheetId="10" r:id="rId3"/>
+    <sheet name="publications" sheetId="3" r:id="rId4"/>
+    <sheet name="presentations" sheetId="4" r:id="rId5"/>
+    <sheet name="mentorship" sheetId="5" r:id="rId6"/>
+    <sheet name="experience" sheetId="6" r:id="rId7"/>
+    <sheet name="affiliations" sheetId="7" r:id="rId8"/>
+    <sheet name="current_work" sheetId="8" r:id="rId9"/>
+    <sheet name="software" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="352">
   <si>
     <t>data</t>
   </si>
@@ -50,18 +51,12 @@
     <t>professor</t>
   </si>
   <si>
-    <t>Fall 2018</t>
-  </si>
-  <si>
     <t>Maps and Spatial Reasoning</t>
   </si>
   <si>
     <t>Dr. Keith Clarke</t>
   </si>
   <si>
-    <t>Summer 2018</t>
-  </si>
-  <si>
     <t>Living with Global Warming</t>
   </si>
   <si>
@@ -71,9 +66,6 @@
     <t>Cartographic Design and Geovisualization</t>
   </si>
   <si>
-    <t>Water Quality</t>
-  </si>
-  <si>
     <t>Conceptual Modeling and Programming for the Geo-Sciences</t>
   </si>
   <si>
@@ -92,33 +84,9 @@
     <t>details</t>
   </si>
   <si>
-    <t>Travel Grant (AGU)</t>
-  </si>
-  <si>
-    <t>Summer Research Grant</t>
-  </si>
-  <si>
     <t>COMET Partners Grant</t>
   </si>
   <si>
-    <t>Seed Grant</t>
-  </si>
-  <si>
-    <t>Travel Scholarship (AGU)</t>
-  </si>
-  <si>
-    <t>National Water Center Course Coordinator</t>
-  </si>
-  <si>
-    <t>Travel Grant (WRF-Hydro Training)</t>
-  </si>
-  <si>
-    <t>Travel Grant (HAZUS Conference)</t>
-  </si>
-  <si>
-    <t>2015-2016</t>
-  </si>
-  <si>
     <t>Disciplines Fellowship</t>
   </si>
   <si>
@@ -126,9 +94,6 @@
   </si>
   <si>
     <t>Cal Poly Department of Geography</t>
-  </si>
-  <si>
-    <t>Top undergraduate paper</t>
   </si>
   <si>
     <t>authors</t>
@@ -335,9 +300,6 @@
     <t>Dec 2018</t>
   </si>
   <si>
-    <t>AGU Fall Meeting</t>
-  </si>
-  <si>
     <t>The National Water Model and R: Providing fast discovery, access, and usability of NWM output and earth systems data</t>
   </si>
   <si>
@@ -362,9 +324,6 @@
     <t>April 2018</t>
   </si>
   <si>
-    <t>EGU</t>
-  </si>
-  <si>
     <t>Integrating Adaption behavior in drought risk analysis</t>
   </si>
   <si>
@@ -416,21 +375,9 @@
     <t>Oct 2016</t>
   </si>
   <si>
-    <t>UCSB SDSU Retreat</t>
-  </si>
-  <si>
     <t>The Five Meanings of Water Security</t>
   </si>
   <si>
-    <t>Aug 2016</t>
-  </si>
-  <si>
-    <t>NCAR</t>
-  </si>
-  <si>
-    <t>FloodHippo and the National Water Model</t>
-  </si>
-  <si>
     <t>July 2016</t>
   </si>
   <si>
@@ -470,24 +417,12 @@
     <t>date</t>
   </si>
   <si>
-    <t>2018-present</t>
-  </si>
-  <si>
     <t>Dino Korac</t>
   </si>
   <si>
-    <t>2016-present</t>
-  </si>
-  <si>
     <t xml:space="preserve">Jeremy Neil	</t>
   </si>
   <si>
-    <t xml:space="preserve">Benjamin Sterne \&amp; Eric Gunter	</t>
-  </si>
-  <si>
-    <t>Spatial Data Science Faculty Search</t>
-  </si>
-  <si>
     <t>UCSB</t>
   </si>
   <si>
@@ -497,24 +432,12 @@
     <t>NCAR Research Applications Laboratory</t>
   </si>
   <si>
-    <t>Winter 2018</t>
-  </si>
-  <si>
-    <t>VU Amsterdam IVM</t>
-  </si>
-  <si>
-    <t>2014-Present</t>
-  </si>
-  <si>
     <t>Certified Agricultural Irrigation Specialist</t>
   </si>
   <si>
     <t>Irrigation Association</t>
   </si>
   <si>
-    <t>Research Coordinator</t>
-  </si>
-  <si>
     <t xml:space="preserve">NOAA National Water Center </t>
   </si>
   <si>
@@ -524,21 +447,9 @@
     <t>El Paso County, Colorado</t>
   </si>
   <si>
-    <t>2014-2015</t>
-  </si>
-  <si>
     <t>Cal Poly Data Studio</t>
   </si>
   <si>
-    <t>San Luis Obispo County</t>
-  </si>
-  <si>
-    <t>Piedras Blancas Mapping and Restoration:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bureau of Land Management: </t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -567,9 +478,6 @@
   </si>
   <si>
     <t>https://geog.ucsb.edu/</t>
-  </si>
-  <si>
-    <t>VU University</t>
   </si>
   <si>
     <t>Amsterdam Netherlands</t>
@@ -900,36 +808,6 @@
     <t>An R Package for flood mapping (HAND &amp; National Water Model)</t>
   </si>
   <si>
-    <t>Graduate Student Association ($200)</t>
-  </si>
-  <si>
-    <t>UCSB Geography ($2,400)</t>
-  </si>
-  <si>
-    <t>UCAR ($15,000)</t>
-  </si>
-  <si>
-    <t>UCGHI Planetary Health Center ($10,000)</t>
-  </si>
-  <si>
-    <t>Dangermond Fund ($800)</t>
-  </si>
-  <si>
-    <t>Dangermond Fund ($700)</t>
-  </si>
-  <si>
-    <t>University of California Regents ($30,000)</t>
-  </si>
-  <si>
-    <t>California Geographical Society ($500)</t>
-  </si>
-  <si>
-    <t>CUAHSI ($15,000)</t>
-  </si>
-  <si>
-    <t>CUAHSI ($500)</t>
-  </si>
-  <si>
     <t>https://github.com/mikejohnson51/nwmRetro</t>
   </si>
   <si>
@@ -993,18 +871,6 @@
     <t>status</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>4</t>
   </si>
   <si>
@@ -1014,94 +880,226 @@
     <t>https://www.nat-hazards-earth-syst-sci-discuss.net/nhess-2019-82/</t>
   </si>
   <si>
-    <t>Spatial Discovery Experts Meeting</t>
-  </si>
-  <si>
     <t>Santa Barbara</t>
   </si>
   <si>
-    <t>May 2019</t>
-  </si>
-  <si>
-    <t>GIS Intern</t>
-  </si>
-  <si>
     <t>GIS Peer Assistant</t>
   </si>
   <si>
-    <t>GIS Technician</t>
-  </si>
-  <si>
     <t>Head Poster Judge - CGS Annual Conference</t>
   </si>
   <si>
-    <t>Research Fellow</t>
-  </si>
-  <si>
-    <t>2019-2020</t>
-  </si>
-  <si>
-    <t>Jack and Laura Dangermond ($5,000)</t>
-  </si>
-  <si>
-    <t>Dangermond GIS Fellow in Residence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Research Grant </t>
-  </si>
-  <si>
-    <t>VU Amsterdam ($2,500)</t>
-  </si>
-  <si>
     <t>An Integrated Evaluation of the National Water Model (NWM) Height Above Nearest Drainage (HAND) Flood Mapping Methodology</t>
   </si>
   <si>
-    <t>Summer 2019</t>
-  </si>
-  <si>
     <t>Journal of Open Source Software</t>
   </si>
   <si>
-    <t>AOI: An R package for converting descriptions of space to formal spatial objects</t>
-  </si>
-  <si>
     <t>The primary functions in this package are are `geocode`, `revgeocode`, `getAOI`, and `getBoundingBox`.  The first returns a data.frame of coordinates from place names using the OSM API; the second returns a list of descriptive features from a known place name or lat/lon pair; the third returns a spatial (sf) geometry from a country, state, county, or defined region, and the last an extent encompassing a set of input features. Additional helper functions include `bbox_st` and `bbox_sp` which help convert AOIs between string and geometries;  `check` which helps users visualize AOIs in an interactive leaflet map; and `modify` which allows AOIs to be modified by uniform distances.  Finally, `describe`  breaks existing spatial features into `getAOI` parameters to improve the reproducibility of geometry generation. Three core datasets are served with the package. The first contains the spatial geometries and attributes of all `world` countries. The second, the spatial geometries for US `states` and the third contains the same for all US `counties`. See the \href{https://github.com/mikejohnson51/AOI/blob/master/README.md}{README} on github, and the project webpage for examples \href{https://mikejohnson51.github.io/AOI/}{here}.</t>
   </si>
   <si>
     <t>Flood maps are needed for emergency response, research, and planning. The Height Above Nearest Drainage (HAND) technique is a low-complexity, terrain-based approach for inundation mapping using elevation data, discharge-height relationships, and streamflow inputs.  The recent operational capacities of the NOAA National Water Model (NWM) and pre-processed HAND products from the University of Texas offer an operational framework for real-time and forecast flood guidance across the United States. In this study, we evaluate the NWM-HAND approach using 28 remotely sensed inundation maps and 54 NHD catchments. The results show the NWM-HAND method tends to underpredict inundated cells in lower order reaches (Strahler order &lt;4) and does better with a slight tendency to over predict, in high order reaches. An evaluation of the roughness coefficient used in the derivation of synthetic rating curves suggests it is the most important parameter for improvement in correcting these errors. Persistent inaccuracies do occur when the NWM misses substantially (&gt;60% mean absolute error between NWM and observed flow) and in regions of low relief. While NWM values are taken as input, suggestions for handling areas of low relief are provided. Overall, the NWM-HAND method does a poor job of accurately capturing inundated cells (~20%) but is quite capable of highlight regions likely to be at risk in fourth order streams and higher. While NWM-HAND should be used with caution when identify flood boundary lines or making decisions predicated of whether a cell is dry or wet, its applicability as a high-level guidance tool along larger rivers is noteworthy.</t>
   </si>
   <si>
-    <t>Dangermond Fund ($500)</t>
-  </si>
-  <si>
     <t>Dr. Hugo Loaiciga</t>
   </si>
   <si>
+    <t>Funds</t>
+  </si>
+  <si>
+    <t>Dangermond Fund</t>
+  </si>
+  <si>
+    <t>Jack and Laura Dangermond</t>
+  </si>
+  <si>
+    <t>Graduate Student Association</t>
+  </si>
+  <si>
+    <t>UCGHI Planetary Health Center</t>
+  </si>
+  <si>
+    <t>University of California Regents</t>
+  </si>
+  <si>
+    <t>AGU</t>
+  </si>
+  <si>
+    <t>WRF-Hydro Training</t>
+  </si>
+  <si>
+    <t>HAZUS Conference</t>
+  </si>
+  <si>
+    <t>class_num</t>
+  </si>
+  <si>
+    <t>class_title</t>
+  </si>
+  <si>
+    <t>class_desc</t>
+  </si>
+  <si>
+    <t>Surveys properties of maps, emphasizing map use and interpretation. Lecture topics include map abstraction, generalization, map projections, and symbolization. Special purpose maps, thematic maps, and the display of quantitative and qualitative information is considered.</t>
+  </si>
+  <si>
+    <t>Overview of global warming and climate change processes. Description of complex relationships between scientific, technological, economic, social, political, and historical facets of global warming and climate change. Introduction to the concept and practice of climate modeling.</t>
+  </si>
+  <si>
+    <t>115C</t>
+  </si>
+  <si>
+    <t>Advanced image processing, including data fusion and resampling techniques, atmospheric corrections, global navigation satellite systems, and hyperspatial sensors with emphasis on applications. Lab is centered around projects (e.g., glacial and vegetation changes in mountain environments) with poster presentation of results.</t>
+  </si>
+  <si>
+    <t>178/258</t>
+  </si>
+  <si>
+    <t>A project-based course introducing major conceptual modeling paradigms and object oriented programming from a Geoinformatics perspective. The class is intended for undergraduate students from Geography and the broader Geo-Sciences who have limited (or no previous) experience in software engineering.</t>
+  </si>
+  <si>
+    <t>Technical introduction to graphic representation and visualization of geographic information. Lectures cover static and dynamic design aspects, thematic mapping, interface design, animation, and 3D. Labs provide experience designing thematic maps and constructing basic GeoVis tools with current software.</t>
+  </si>
+  <si>
+    <t>Environmental Water Quality</t>
+  </si>
+  <si>
+    <t>Study of physio-chemical and biological characteristics of natural waters, analysis of water pollution and treatment, water-quality regulations. Laboratory: independent and supervised research on water pollutants and treatment, quantitative analysis of water-quality data and one-day field work.</t>
+  </si>
+  <si>
+    <t>Introduction to the oceans and atmosphere and their role in the Earth's climate and its weather patterns. Focus on the flows of solar energy through the ocean and atmosphere systems. Human impacts of the Earth's climate are also introduced.</t>
+  </si>
+  <si>
+    <t>quarter</t>
+  </si>
+  <si>
+    <t>Fall</t>
+  </si>
+  <si>
     <t>Lower-Division</t>
   </si>
   <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
     <t>Upper-Division</t>
   </si>
   <si>
+    <t>Winter</t>
+  </si>
+  <si>
     <t>Upper-Division and Graduate</t>
   </si>
   <si>
-    <t>quarter</t>
-  </si>
-  <si>
-    <t>Fall</t>
-  </si>
-  <si>
-    <t>Summer</t>
-  </si>
-  <si>
-    <t>Spring</t>
-  </si>
-  <si>
-    <t>Winter</t>
-  </si>
-  <si>
     <t>https://github.com/mikejohnson51/geog178</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>Summer Institute Course Coordinator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visting Scholar Research Grant </t>
+  </si>
+  <si>
+    <t>Summer Support Research Grant</t>
+  </si>
+  <si>
+    <t>UC Global Health Institute Seed Grant</t>
+  </si>
+  <si>
+    <t>Summer Instistute Research Fellow</t>
+  </si>
+  <si>
+    <t>Spatial Discovery Experts Meeting Attendee</t>
+  </si>
+  <si>
+    <t>Spatial Data Science Faculty Search Committee</t>
+  </si>
+  <si>
+    <t>County GIS Technician</t>
+  </si>
+  <si>
+    <t>County GIS Intern</t>
+  </si>
+  <si>
+    <t>San Luis Obispo County, California</t>
+  </si>
+  <si>
+    <t>Piedras Blancas Mapping and Restoration Project</t>
+  </si>
+  <si>
+    <t>Bureau of Land Management / Cal Poly</t>
+  </si>
+  <si>
+    <t>2014 - 2015</t>
+  </si>
+  <si>
+    <t>2014 - 2019</t>
+  </si>
+  <si>
+    <t>In Review</t>
+  </si>
+  <si>
+    <t>Peer-Reviewed Journal Papers</t>
+  </si>
+  <si>
+    <t>Technical Reports</t>
+  </si>
+  <si>
+    <t>Cartography</t>
+  </si>
+  <si>
+    <t>AOI: An R package for fast and flexible geocoding, boundary query, and AOI generation</t>
+  </si>
+  <si>
+    <t>Benjamin Sterne, Eric Gunter</t>
+  </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/doi/full/10.1002/wat2.1345</t>
+  </si>
+  <si>
+    <t>https://github.com/mikejohnson51/AOI/blob/master/paper/output/2019-09-06_paper.pdf</t>
+  </si>
+  <si>
+    <t>Travel Grants</t>
+  </si>
+  <si>
+    <t>Grants, Fellowships, Awards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vrije Universiteit Amsterdam </t>
+  </si>
+  <si>
+    <t>Vrije Universiteit Amsterdam</t>
+  </si>
+  <si>
+    <t>Vrije Universiteit University</t>
+  </si>
+  <si>
+    <t>American Geophysical Union</t>
+  </si>
+  <si>
+    <t>Jack &amp; Laura Dangermond Fellowship</t>
+  </si>
+  <si>
+    <t>Top Undergraduate Paper</t>
+  </si>
+  <si>
+    <t>UCAR/NOAA National Water Center</t>
+  </si>
+  <si>
+    <t>American Geophysical Union Fall Meeting</t>
+  </si>
+  <si>
+    <t>European Geophysical Union</t>
+  </si>
+  <si>
+    <t>UCSB-SDSU Retreat</t>
   </si>
 </sst>
 </file>
@@ -1184,9 +1182,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1206,9 +1203,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1595,26 +1600,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="44" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView zoomScale="106" zoomScaleNormal="44" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="52.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="39" bestFit="1" customWidth="1"/>
-    <col min="7" max="1025" width="10.5" customWidth="1"/>
+    <col min="6" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>347</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>308</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1623,226 +1628,475 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="F1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>348</v>
+        <v>309</v>
       </c>
       <c r="B2">
         <v>2019</v>
       </c>
       <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
       <c r="E2" t="s">
-        <v>344</v>
+        <v>310</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>349</v>
-      </c>
-      <c r="B3" s="6">
+        <v>311</v>
+      </c>
+      <c r="B3">
         <v>2019</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>344</v>
+        <v>310</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>350</v>
+        <v>312</v>
       </c>
       <c r="B4">
         <v>2019</v>
       </c>
       <c r="C4" t="s">
-        <v>311</v>
+        <v>270</v>
       </c>
       <c r="D4" t="s">
-        <v>312</v>
+        <v>271</v>
       </c>
       <c r="E4" t="s">
-        <v>345</v>
+        <v>313</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>351</v>
+        <v>314</v>
       </c>
       <c r="B5">
         <v>2019</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>321</v>
+        <v>276</v>
       </c>
       <c r="E5" t="s">
-        <v>346</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>352</v>
+        <v>315</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>348</v>
+        <v>309</v>
       </c>
       <c r="B6">
         <v>2018</v>
       </c>
       <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
       <c r="E6" t="s">
-        <v>344</v>
+        <v>310</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>349</v>
+        <v>311</v>
       </c>
       <c r="B7">
         <v>2018</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>344</v>
+        <v>310</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>350</v>
+        <v>312</v>
       </c>
       <c r="B8">
         <v>2018</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>345</v>
+        <v>313</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>348</v>
+        <v>309</v>
       </c>
       <c r="B9">
         <v>2017</v>
       </c>
       <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
         <v>4</v>
       </c>
-      <c r="D9" t="s">
-        <v>5</v>
-      </c>
       <c r="E9" t="s">
-        <v>344</v>
+        <v>310</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>350</v>
+        <v>312</v>
       </c>
       <c r="B10">
         <v>2017</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>305</v>
       </c>
       <c r="D10" t="s">
-        <v>343</v>
+        <v>285</v>
       </c>
       <c r="E10" t="s">
-        <v>345</v>
+        <v>313</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>351</v>
+        <v>314</v>
       </c>
       <c r="B11">
         <v>2017</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>321</v>
+        <v>276</v>
       </c>
       <c r="E11" t="s">
-        <v>346</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>352</v>
+        <v>315</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>348</v>
+        <v>309</v>
       </c>
       <c r="B12">
         <v>2016</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>344</v>
+        <v>310</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>349</v>
+        <v>311</v>
       </c>
       <c r="B13">
         <v>2016</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>344</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F5" r:id="rId1" xr:uid="{B4C354B1-6171-3742-8B79-F4256809C196}"/>
-    <hyperlink ref="F11" r:id="rId2" xr:uid="{D0AF7623-6AA9-8B43-86CA-D56E8999CE59}"/>
+    <hyperlink ref="F5" r:id="rId1" xr:uid="{2712DA81-3E6F-694E-BA29-B446F68F2C4C}"/>
+    <hyperlink ref="F11" r:id="rId2" xr:uid="{10422249-9E5C-FB4C-BC18-65775B4398EE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.5" style="9" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="55" style="9" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="34" style="9" customWidth="1"/>
+    <col min="7" max="7" width="39.6640625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="37.6640625" style="9" customWidth="1"/>
+    <col min="9" max="9" width="46.83203125" style="9" customWidth="1"/>
+    <col min="10" max="1025" width="10.5" style="9" customWidth="1"/>
+    <col min="1026" max="16384" width="8.83203125" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="404" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="306" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="306" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="153" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="204" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>249</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G5" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="G6" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="G7" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1851,183 +2105,255 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView zoomScale="108" zoomScaleNormal="44" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E17"/>
+    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="44" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.83203125" customWidth="1"/>
     <col min="2" max="2" width="41.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36" customWidth="1"/>
-    <col min="4" max="1025" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="41.1640625" customWidth="1"/>
+    <col min="4" max="4" width="36" customWidth="1"/>
+    <col min="5" max="5" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="1026" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>286</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2019</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>331</v>
+        <v>292</v>
+      </c>
+      <c r="C2">
+        <v>500</v>
+      </c>
+      <c r="D2" t="s">
+        <v>287</v>
+      </c>
+      <c r="E2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2019</v>
       </c>
       <c r="B3" t="s">
-        <v>333</v>
-      </c>
-      <c r="C3" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>346</v>
+      </c>
+      <c r="C3">
+        <v>5000</v>
+      </c>
+      <c r="D3" t="s">
+        <v>288</v>
+      </c>
+      <c r="E3" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2019</v>
       </c>
       <c r="B4" t="s">
-        <v>334</v>
-      </c>
-      <c r="C4" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>319</v>
+      </c>
+      <c r="C4">
+        <v>2500</v>
+      </c>
+      <c r="D4" t="s">
+        <v>342</v>
+      </c>
+      <c r="E4" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2018</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+      <c r="C5">
+        <v>200</v>
+      </c>
+      <c r="D5" t="s">
+        <v>289</v>
+      </c>
+      <c r="E5" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2018</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>320</v>
+      </c>
+      <c r="C6">
+        <v>2400</v>
+      </c>
+      <c r="D6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E6" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2018</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>15000</v>
+      </c>
+      <c r="D7" t="s">
+        <v>348</v>
+      </c>
+      <c r="E7" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2017</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>321</v>
+      </c>
+      <c r="C8">
+        <v>10000</v>
+      </c>
+      <c r="D8" t="s">
+        <v>290</v>
+      </c>
+      <c r="E8" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2017</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+      <c r="C9">
+        <v>800</v>
+      </c>
+      <c r="D9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E9" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2017</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>500</v>
+      </c>
+      <c r="D10" t="s">
+        <v>257</v>
+      </c>
+      <c r="E10" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>700</v>
+      </c>
+      <c r="D11" t="s">
+        <v>287</v>
+      </c>
+      <c r="E11" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>25</v>
+        <v>15</v>
+      </c>
+      <c r="C12">
+        <v>30000</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="E12" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2015</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2015</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>2015</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" t="s">
-        <v>292</v>
+        <v>347</v>
+      </c>
+      <c r="C14">
+        <v>500</v>
+      </c>
+      <c r="D14" t="s">
+        <v>132</v>
+      </c>
+      <c r="E14" t="s">
+        <v>341</v>
       </c>
     </row>
   </sheetData>
@@ -2037,11 +2363,118 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3445A971-4551-0848-B274-DFAE26C643B4}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="52.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="255.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="15">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="15">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="B4" t="s">
+        <v>270</v>
+      </c>
+      <c r="C4" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="15">
+        <v>183</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="15">
+        <v>162</v>
+      </c>
+      <c r="B7" t="s">
+        <v>305</v>
+      </c>
+      <c r="C7" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="15">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>307</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView topLeftCell="F1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2053,434 +2486,442 @@
     <col min="6" max="6" width="63.6640625" customWidth="1"/>
     <col min="7" max="7" width="38.6640625" customWidth="1"/>
     <col min="8" max="8" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="255.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="255.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.5" customWidth="1"/>
     <col min="11" max="1026" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>315</v>
+      <c r="A1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>274</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="G1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="H1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>36</v>
+        <v>23</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="J1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="K1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="70" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>316</v>
+      <c r="A2" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>332</v>
       </c>
       <c r="C2">
         <v>2019</v>
       </c>
       <c r="D2" t="s">
-        <v>336</v>
+        <v>281</v>
       </c>
       <c r="E2" t="s">
-        <v>308</v>
+        <v>267</v>
       </c>
       <c r="F2" t="s">
-        <v>322</v>
-      </c>
-      <c r="I2" s="16" t="s">
-        <v>341</v>
+        <v>277</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>316</v>
+      <c r="A3" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>332</v>
       </c>
       <c r="C3">
         <v>2019</v>
       </c>
       <c r="D3" t="s">
+        <v>336</v>
+      </c>
+      <c r="E3" t="s">
+        <v>282</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>339</v>
       </c>
-      <c r="E3" t="s">
-        <v>338</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="I3" s="16" t="s">
-        <v>340</v>
+      <c r="G3" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>316</v>
+      <c r="A4" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>332</v>
       </c>
       <c r="C4">
         <v>2019</v>
       </c>
       <c r="D4" t="s">
-        <v>309</v>
+        <v>268</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="28" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>310</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>317</v>
+      <c r="A5" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>333</v>
       </c>
       <c r="C5">
         <v>2019</v>
       </c>
       <c r="D5" t="s">
-        <v>305</v>
+        <v>264</v>
       </c>
       <c r="E5" t="s">
-        <v>306</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>46</v>
+        <v>265</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="56" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>317</v>
+      <c r="A6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>333</v>
       </c>
       <c r="C6">
         <v>2019</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>301</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>302</v>
+      <c r="D6" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>261</v>
       </c>
       <c r="H6" t="s">
-        <v>304</v>
-      </c>
-      <c r="I6" s="16" t="s">
-        <v>41</v>
+        <v>263</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="42" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>320</v>
+      <c r="A7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>275</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>303</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="J7" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:11" ht="42" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>317</v>
+      <c r="A8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>333</v>
       </c>
       <c r="C8">
         <v>2018</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="F8" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="H8" t="s">
-        <v>51</v>
-      </c>
-      <c r="I8" s="16" t="s">
-        <v>52</v>
+        <v>39</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="56" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>317</v>
+      <c r="A9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>333</v>
       </c>
       <c r="C9">
         <v>2018</v>
       </c>
       <c r="D9" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F9" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G9" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="H9" t="s">
-        <v>58</v>
-      </c>
-      <c r="I9" s="16" t="s">
-        <v>59</v>
+        <v>46</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="42" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>317</v>
+      <c r="A10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>333</v>
       </c>
       <c r="C10">
         <v>2017</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="E10" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F10" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="G10" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="H10" t="s">
-        <v>64</v>
-      </c>
-      <c r="I10" s="16" t="s">
-        <v>65</v>
+        <v>52</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="42" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>318</v>
+      <c r="A11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>334</v>
       </c>
       <c r="C11">
         <v>2017</v>
       </c>
       <c r="D11" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E11" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="F11" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="H11" t="s">
-        <v>51</v>
-      </c>
-      <c r="I11" s="16" t="s">
-        <v>70</v>
+        <v>39</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>319</v>
+      <c r="A12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>335</v>
       </c>
       <c r="C12">
         <v>2017</v>
       </c>
       <c r="D12" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E12" t="s">
-        <v>73</v>
-      </c>
-      <c r="I12" s="16"/>
+        <v>61</v>
+      </c>
+      <c r="I12" s="14"/>
       <c r="J12" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="K12" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>319</v>
+      <c r="A13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>335</v>
       </c>
       <c r="C13">
         <v>2017</v>
       </c>
       <c r="D13" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="E13" t="s">
-        <v>77</v>
-      </c>
-      <c r="I13" s="16"/>
+        <v>65</v>
+      </c>
+      <c r="I13" s="14"/>
       <c r="J13" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="K13" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>319</v>
+      <c r="A14" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>335</v>
       </c>
       <c r="C14">
         <v>2017</v>
       </c>
       <c r="D14" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="E14" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="F14" t="s">
-        <v>82</v>
-      </c>
-      <c r="I14" s="16"/>
+        <v>70</v>
+      </c>
+      <c r="I14" s="14"/>
       <c r="J14" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="K14" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>318</v>
+      <c r="A15" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>334</v>
       </c>
       <c r="C15">
         <v>2016</v>
       </c>
       <c r="D15" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="E15" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="F15" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="H15" t="s">
-        <v>89</v>
-      </c>
-      <c r="I15" s="16" t="s">
-        <v>90</v>
+        <v>77</v>
+      </c>
+      <c r="I15" s="14" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="56" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>318</v>
+      <c r="A16" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>334</v>
       </c>
       <c r="C16">
         <v>2016</v>
       </c>
       <c r="D16" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="E16" t="s">
-        <v>314</v>
+        <v>273</v>
       </c>
       <c r="F16" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="H16" t="s">
-        <v>89</v>
-      </c>
-      <c r="I16" s="16" t="s">
-        <v>93</v>
+        <v>77</v>
+      </c>
+      <c r="I16" s="14" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F7" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
     <hyperlink ref="G3" r:id="rId2" xr:uid="{EDB1E5CE-989F-A048-AB3F-B8DDD1C9772C}"/>
+    <hyperlink ref="F5" r:id="rId3" xr:uid="{4AB00A8A-D1C4-F44D-BEC6-4EE1437F4BF9}"/>
+    <hyperlink ref="F3" r:id="rId4" xr:uid="{D99F2ED0-AF0F-FB47-9F40-A04876AB15FE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="114" zoomScaleNormal="44" workbookViewId="0">
-      <selection activeCell="B2" sqref="A2:XFD2"/>
+    <sheetView zoomScale="114" zoomScaleNormal="44" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.5" style="4" customWidth="1"/>
+    <col min="1" max="1" width="9.5" style="3" customWidth="1"/>
     <col min="2" max="2" width="55.83203125" customWidth="1"/>
     <col min="3" max="3" width="101.83203125" customWidth="1"/>
     <col min="4" max="4" width="20.83203125" customWidth="1"/>
@@ -2488,248 +2929,234 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
+        <v>349</v>
+      </c>
+      <c r="C3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" t="s">
+        <v>350</v>
+      </c>
+      <c r="C6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" t="s">
         <v>94</v>
       </c>
-      <c r="C1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="B7" t="s">
+        <v>349</v>
+      </c>
+      <c r="C7" t="s">
         <v>96</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D7" t="s">
         <v>97</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B8" t="s">
+        <v>255</v>
+      </c>
+      <c r="C8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="D9" t="s">
         <v>100</v>
       </c>
-      <c r="B4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" t="s">
-        <v>102</v>
-      </c>
-      <c r="D4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="B10" t="s">
         <v>105</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C10" t="s">
         <v>106</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B11" t="s">
         <v>107</v>
       </c>
-      <c r="D6" t="s">
+      <c r="C11" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="D11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B12" t="s">
+        <v>351</v>
+      </c>
+      <c r="C12" t="s">
         <v>110</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="B13" t="s">
+        <v>256</v>
+      </c>
+      <c r="C13" t="s">
         <v>112</v>
       </c>
-      <c r="B8" t="s">
-        <v>296</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="D13" t="s">
         <v>113</v>
       </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="B14" t="s">
         <v>115</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C14" t="s">
         <v>116</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D14" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D9" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="B15" t="s">
         <v>118</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C15" t="s">
         <v>119</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="B16" t="s">
         <v>121</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C16" t="s">
         <v>122</v>
       </c>
-      <c r="D11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B12" t="s">
-        <v>124</v>
-      </c>
-      <c r="C12" t="s">
-        <v>125</v>
-      </c>
-      <c r="D12" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B13" t="s">
-        <v>127</v>
-      </c>
-      <c r="C13" t="s">
-        <v>128</v>
-      </c>
-      <c r="D13" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="B14" t="s">
-        <v>297</v>
-      </c>
-      <c r="C14" t="s">
-        <v>130</v>
-      </c>
-      <c r="D14" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B15" t="s">
-        <v>133</v>
-      </c>
-      <c r="C15" t="s">
-        <v>134</v>
-      </c>
-      <c r="D15" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B16" t="s">
-        <v>136</v>
-      </c>
-      <c r="C16" t="s">
-        <v>137</v>
-      </c>
       <c r="D16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="B17" t="s">
-        <v>139</v>
-      </c>
-      <c r="C17" t="s">
-        <v>140</v>
-      </c>
-      <c r="D17" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="B25" s="7"/>
-    </row>
-    <row r="27" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="B27" s="7"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="B24" s="6"/>
+    </row>
+    <row r="26" spans="2:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="B26" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -2737,12 +3164,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
-      <selection activeCellId="1" sqref="I8 A1"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2754,34 +3181,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>142</v>
+      <c r="A2">
+        <v>2018</v>
       </c>
       <c r="B2" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>144</v>
+      <c r="A3">
+        <v>2017</v>
       </c>
       <c r="B3" t="s">
-        <v>145</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2790,18 +3217,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView zoomScale="156" zoomScaleNormal="44" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
-    <col min="2" max="2" width="37.5" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.33203125" customWidth="1"/>
     <col min="4" max="1025" width="10.5" customWidth="1"/>
   </cols>
@@ -2811,153 +3238,153 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>337</v>
+      <c r="A2" s="16">
+        <v>2019</v>
       </c>
       <c r="B2" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="C2" t="s">
-        <v>152</v>
+        <v>343</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
-        <v>325</v>
+      <c r="A3" s="17" t="s">
+        <v>317</v>
       </c>
       <c r="B3" t="s">
         <v>323</v>
       </c>
       <c r="C3" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="16">
+        <v>2018</v>
+      </c>
+      <c r="B4" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>147</v>
-      </c>
       <c r="C4" t="s">
-        <v>148</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>6</v>
+      <c r="A5" s="16">
+        <v>2018</v>
       </c>
       <c r="B5" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="C5" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>151</v>
+      <c r="A6" s="16">
+        <v>2018</v>
       </c>
       <c r="B6" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="C6" t="s">
-        <v>152</v>
+        <v>342</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>153</v>
+      <c r="A7" s="16">
+        <v>2017</v>
       </c>
       <c r="B7" t="s">
-        <v>154</v>
+        <v>318</v>
       </c>
       <c r="C7" t="s">
-        <v>155</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>2017</v>
+      <c r="A8" s="16">
+        <v>2016</v>
       </c>
       <c r="B8" t="s">
-        <v>156</v>
+        <v>322</v>
       </c>
       <c r="C8" t="s">
-        <v>157</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="16">
         <v>2016</v>
       </c>
       <c r="B9" t="s">
+        <v>280</v>
+      </c>
+      <c r="C9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="16">
+        <v>2015</v>
+      </c>
+      <c r="B10" t="s">
+        <v>325</v>
+      </c>
+      <c r="C10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="16" t="s">
         <v>330</v>
       </c>
-      <c r="C9" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>2016</v>
-      </c>
-      <c r="B10" t="s">
-        <v>329</v>
-      </c>
-      <c r="C10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>2015</v>
-      </c>
       <c r="B11" t="s">
-        <v>328</v>
+        <v>279</v>
       </c>
       <c r="C11" t="s">
-        <v>159</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>160</v>
+      <c r="A12" s="16" t="s">
+        <v>331</v>
       </c>
       <c r="B12" t="s">
-        <v>327</v>
+        <v>129</v>
       </c>
       <c r="C12" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="A13" s="16">
         <v>2014</v>
       </c>
       <c r="B13" t="s">
         <v>326</v>
       </c>
       <c r="C13" t="s">
-        <v>162</v>
+        <v>327</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="A14" s="16">
         <v>2013</v>
       </c>
       <c r="B14" t="s">
-        <v>163</v>
+        <v>328</v>
       </c>
       <c r="C14" t="s">
-        <v>164</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -2966,254 +3393,254 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView zoomScale="44" zoomScaleNormal="44" workbookViewId="0">
-      <selection activeCell="B3" activeCellId="1" sqref="I8 B3"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.83203125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="22.83203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="8.1640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="36" style="4" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="38.6640625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="24.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="36" style="3" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="38.6640625" style="3" customWidth="1"/>
     <col min="8" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" s="3">
+        <v>-119.845</v>
+      </c>
+      <c r="D2" s="3">
+        <v>34.414999999999999</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F2" s="3">
+        <v>75</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C3" s="3">
+        <v>4.8657000000000004</v>
+      </c>
+      <c r="D3" s="3">
+        <v>52.333799999999997</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="F3" s="3">
+        <v>75</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C4" s="3">
+        <v>-71.109700000000004</v>
+      </c>
+      <c r="D4" s="3">
+        <v>42.373600000000003</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="F4" s="3">
+        <v>50</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C5" s="3">
+        <v>-77.306399999999996</v>
+      </c>
+      <c r="D5" s="3">
+        <v>38.846200000000003</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F5" s="3">
+        <v>75</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C6" s="3">
+        <v>-87.541399999999996</v>
+      </c>
+      <c r="D6" s="3">
+        <v>33.217599999999997</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F6" s="3">
+        <v>50</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C7" s="3">
+        <v>-105.27500000000001</v>
+      </c>
+      <c r="D7" s="3">
+        <v>39.978299999999997</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="F7" s="3">
+        <v>50</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C8" s="3">
+        <v>-122.4586</v>
+      </c>
+      <c r="D8" s="3">
+        <v>37.762700000000002</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="F8" s="3">
+        <v>75</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C9" s="3">
+        <v>-122.2711</v>
+      </c>
+      <c r="D9" s="3">
+        <v>37.804400000000001</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F9" s="3">
+        <v>50</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="E1" s="4" t="s">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="C10" s="3">
+        <v>-120.66249999999999</v>
+      </c>
+      <c r="D10" s="3">
+        <v>35.305</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="F10" s="3">
+        <v>50</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>172</v>
-      </c>
-      <c r="C2" s="4">
-        <v>-119.845</v>
-      </c>
-      <c r="D2" s="4">
-        <v>34.414999999999999</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="F2" s="4">
-        <v>75</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="C3" s="4">
-        <v>4.8657000000000004</v>
-      </c>
-      <c r="D3" s="4">
-        <v>52.333799999999997</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="F3" s="4">
-        <v>75</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="C4" s="4">
-        <v>-71.109700000000004</v>
-      </c>
-      <c r="D4" s="4">
-        <v>42.373600000000003</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>299</v>
-      </c>
-      <c r="F4" s="4">
-        <v>50</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="C5" s="4">
-        <v>-77.306399999999996</v>
-      </c>
-      <c r="D5" s="4">
-        <v>38.846200000000003</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="F5" s="4">
-        <v>75</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="C6" s="4">
-        <v>-87.541399999999996</v>
-      </c>
-      <c r="D6" s="4">
-        <v>33.217599999999997</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="F6" s="4">
-        <v>50</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="C7" s="4">
-        <v>-105.27500000000001</v>
-      </c>
-      <c r="D7" s="4">
-        <v>39.978299999999997</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="F7" s="4">
-        <v>50</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="C8" s="4">
-        <v>-122.4586</v>
-      </c>
-      <c r="D8" s="4">
-        <v>37.762700000000002</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="F8" s="4">
-        <v>75</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="C9" s="4">
-        <v>-122.2711</v>
-      </c>
-      <c r="D9" s="4">
-        <v>37.804400000000001</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="F9" s="4">
-        <v>50</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="C10" s="4">
-        <v>-120.66249999999999</v>
-      </c>
-      <c r="D10" s="4">
-        <v>35.305</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="F10" s="4">
-        <v>50</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -3225,7 +3652,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -3239,357 +3666,108 @@
     <col min="2" max="2" width="55" customWidth="1"/>
     <col min="3" max="3" width="36" customWidth="1"/>
     <col min="4" max="4" width="42" customWidth="1"/>
-    <col min="5" max="5" width="55" style="9" customWidth="1"/>
+    <col min="5" max="5" width="55" style="8" customWidth="1"/>
     <col min="6" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>204</v>
+        <v>173</v>
       </c>
       <c r="B1" t="s">
-        <v>205</v>
+        <v>174</v>
       </c>
       <c r="C1" t="s">
-        <v>206</v>
+        <v>175</v>
       </c>
       <c r="D1" t="s">
-        <v>207</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>208</v>
+        <v>176</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="153" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>209</v>
+        <v>178</v>
       </c>
       <c r="B2" t="s">
-        <v>210</v>
+        <v>179</v>
       </c>
       <c r="C2" t="s">
-        <v>211</v>
+        <v>180</v>
       </c>
       <c r="D2" t="s">
-        <v>212</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>213</v>
+        <v>181</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="170" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>214</v>
+        <v>183</v>
       </c>
       <c r="C3" t="s">
-        <v>215</v>
+        <v>184</v>
       </c>
       <c r="D3" t="s">
-        <v>216</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>217</v>
+        <v>185</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>218</v>
+        <v>187</v>
       </c>
       <c r="B4" t="s">
-        <v>219</v>
+        <v>188</v>
       </c>
       <c r="C4" t="s">
-        <v>220</v>
+        <v>189</v>
       </c>
       <c r="D4" t="s">
-        <v>221</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>222</v>
+        <v>190</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>223</v>
+        <v>192</v>
       </c>
       <c r="C5" t="s">
-        <v>220</v>
+        <v>189</v>
       </c>
       <c r="D5" t="s">
-        <v>224</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>225</v>
+        <v>193</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>226</v>
+        <v>195</v>
       </c>
       <c r="B6" t="s">
-        <v>227</v>
+        <v>196</v>
       </c>
       <c r="C6" t="s">
-        <v>228</v>
+        <v>197</v>
       </c>
       <c r="D6" t="s">
-        <v>229</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>230</v>
+        <v>198</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:I10"/>
-  <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="13.5" style="10" customWidth="1"/>
-    <col min="2" max="2" width="24.1640625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="55" style="10" customWidth="1"/>
-    <col min="5" max="5" width="19.83203125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="34" style="10" customWidth="1"/>
-    <col min="7" max="7" width="39.6640625" style="10" customWidth="1"/>
-    <col min="8" max="8" width="37.6640625" style="10" customWidth="1"/>
-    <col min="9" max="9" width="46.83203125" style="10" customWidth="1"/>
-    <col min="10" max="1025" width="10.5" style="10" customWidth="1"/>
-    <col min="1026" max="16384" width="8.83203125" style="10"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
-        <v>234</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>239</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="404" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>241</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>242</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>243</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>244</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>245</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="306" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
-        <v>247</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>248</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>249</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>250</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>251</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>253</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="306" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
-        <v>254</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>255</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>256</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>258</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="153" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
-        <v>260</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>261</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>283</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
-        <v>264</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>265</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>266</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="204" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
-        <v>268</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>284</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>270</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>271</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>274</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>249</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>295</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
-        <v>275</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>276</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>249</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>278</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>279</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>280</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G5" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
-    <hyperlink ref="G6" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
-    <hyperlink ref="G7" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
 </file>
</xml_diff>